<commit_message>
feat (app): add B type of work and prod verion in dist
</commit_message>
<xml_diff>
--- a/input/Check.xlsx
+++ b/input/Check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\matrixBert\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC0B4F6-B123-4246-9AF6-15763D03B394}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7089C5-D189-4FD4-A7EE-670C5B221F48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -379,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,6 +1149,2502 @@
         <v>1</v>
       </c>
     </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>1</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>1</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>1</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="J95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>1</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>1</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>1</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>1</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>1</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:F1"/>

</xml_diff>